<commit_message>
Import Employee as User
</commit_message>
<xml_diff>
--- a/public/DataEmployee/custom_employee_template (1).xlsx
+++ b/public/DataEmployee/custom_employee_template (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acha\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15985EB9-C754-4B78-94FD-4F1ADD7CFCB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85F10F6-7BB9-4AD4-A414-DE2AC6ED9D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,70 +31,52 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
-  <si>
-    <t>Keterangan: Silakan isi data pegawai sesuai dengan format yang diberikan di bawah ini</t>
-  </si>
-  <si>
-    <t>Kolom A</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t>Nama Pegawai</t>
   </si>
   <si>
-    <t>Kolom B</t>
-  </si>
-  <si>
     <t>Divisi</t>
   </si>
   <si>
+    <t>NIP</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Pangkat</t>
+  </si>
+  <si>
+    <t>mutia</t>
+  </si>
+  <si>
     <t>Produksi</t>
   </si>
   <si>
-    <t>Sosial</t>
-  </si>
-  <si>
-    <t>Distribusi</t>
-  </si>
-  <si>
-    <t>IPDS</t>
-  </si>
-  <si>
-    <t>Neraca</t>
-  </si>
-  <si>
-    <t>Kolom C</t>
-  </si>
-  <si>
-    <t>NIP</t>
-  </si>
-  <si>
-    <t>Kolom D</t>
-  </si>
-  <si>
-    <t>Email Registrasi</t>
-  </si>
-  <si>
-    <t>Kolom E</t>
-  </si>
-  <si>
-    <t>Pangkat</t>
-  </si>
-  <si>
-    <t>zakia</t>
-  </si>
-  <si>
-    <t>kepala</t>
+    <t>mutia@bps.go.id</t>
+  </si>
+  <si>
+    <t>sekretaris</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -115,13 +97,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -424,120 +409,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1">
         <v>1</v>
       </c>
-      <c r="D1">
-        <v>123</v>
-      </c>
-      <c r="E1">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="M2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="M4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="M5" t="s">
-        <v>3</v>
-      </c>
-      <c r="N5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="M7">
-        <v>2</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="M8">
-        <v>3</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="M9">
-        <v>4</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="D2">
+        <v>12345</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="M10">
-        <v>5</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="F2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="M11" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="M12" t="s">
-        <v>12</v>
-      </c>
-      <c r="N12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="M13" t="s">
-        <v>14</v>
-      </c>
-      <c r="N13" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{B18113FE-CB55-4724-91D2-2BEBEAAE2238}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>